<commit_message>
Final cleanup: Project core stable and secrets removed
</commit_message>
<xml_diff>
--- a/unified_analytics.xlsx
+++ b/unified_analytics.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <col width="50" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="13" customWidth="1" min="3" max="3"/>
-    <col width="24" customWidth="1" min="4" max="4"/>
+    <col width="32" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -507,45 +507,45 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TechCorp Solutions</t>
+          <t>BotFather</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>125500</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sample_report_1.txt</t>
+          <t>BotFather.txt</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>format_b</t>
+          <t>format_a</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GlobalTrade Inc</t>
+          <t>TechCorp Solutions</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>125500</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>sample_report_2.txt</t>
+          <t>sample_report_1.txt</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -557,20 +557,20 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>was particularly concerned about compliance and integration with their existing Salesforce setup.</t>
+          <t>GlobalTrade Inc</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>87300</v>
+        <v>0</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>sample_report_3.txt</t>
+          <t>sample_report_2.txt</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -582,7 +582,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Telegram</t>
+          <t>was particularly concerned about compliance and integration with their existing Salesforce setup.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -591,23 +591,23 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>87300</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Telegram.txt</t>
+          <t>sample_report_3.txt</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>format_a</t>
+          <t>format_b</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>UFO</t>
+          <t>Send_Message_telegram</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -620,7 +620,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>UFO.txt</t>
+          <t>Send_Message_telegram.txt</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -632,7 +632,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ілля</t>
+          <t>Telegram</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -645,10 +645,85 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>Telegram.txt</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>format_a</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>UFO</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>UFO.txt</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>format_a</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>User Info • Get ID • idbot</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>User Info • Get ID • idbot.txt</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>format_a</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ілля</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>500</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>Ілля.txt</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>format_a</t>
         </is>
@@ -676,7 +751,7 @@
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
@@ -715,22 +790,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>42.85714285714285</v>
+        <v>20</v>
       </c>
       <c r="E2" t="n">
         <v>212800</v>
       </c>
       <c r="F2" t="n">
-        <v>70933.33333333333</v>
+        <v>106400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>